<commit_message>
Dizili arama denendi pişman olundu
</commit_message>
<xml_diff>
--- a/p ve max tahminleri.xlsx
+++ b/p ve max tahminleri.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3A631A7-CF16-4106-AD87-20AD87826399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F08C6DC2-DB60-48E4-8391-7BE2E2977E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,6 +33,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
+    <t>Reel demek şimdiye kadar bulunmuş en iyi sonuç olan ancak opitmum olmaması muhtemel olan sonuç</t>
+  </si>
+  <si>
     <t>p</t>
   </si>
   <si>
@@ -57,19 +60,16 @@
     <t>m/p</t>
   </si>
   <si>
-    <t>Kişisel Tahmin</t>
-  </si>
-  <si>
     <t>max ve reel</t>
   </si>
   <si>
     <t>----??&gt;</t>
   </si>
   <si>
-    <t>SONUÇ= 9 İÇİN MUHTEMELEN 64 ÇIKACAK</t>
+    <t>SONUÇ= 9 İÇİN 66-63 arası muhtemel 64</t>
   </si>
   <si>
-    <t>10 İÇİN 73-78 ARASI 76 ÇIKACAK GİBİ</t>
+    <t>10 İÇİN 76-78 ARASI muhtemel 76</t>
   </si>
 </sst>
 </file>
@@ -1450,25 +1450,46 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="7"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:trendlineType val="linear"/>
             <c:forward val="7"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.1803358650965094E-2"/>
+                  <c:y val="-0.13467592592592592"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:trendline>
             <c:spPr>
@@ -1483,8 +1504,44 @@
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:forward val="7"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.8919471349267176E-2"/>
+                  <c:y val="0.28522783610382035"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:cat>
             <c:numRef>
@@ -1846,51 +1903,6 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
             <c:name>3.D</c:name>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -1907,6 +1919,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.3926852743022133E-3"/>
+                  <c:y val="0.2791766654168229"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1983,20 +2001,6 @@
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
           </c:trendline>
           <c:yVal>
             <c:numRef>
@@ -5548,16 +5552,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5944,10 +5948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AA38"/>
+  <dimension ref="B1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5958,32 +5962,34 @@
     <col min="27" max="27" width="11" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:27">
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="2:27">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" t="s">
         <v>8</v>
       </c>
       <c r="AA2" t="s">
@@ -6589,7 +6595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="19:22">
+    <row r="37" spans="19:21">
       <c r="S37">
         <v>9</v>
       </c>
@@ -6601,12 +6607,8 @@
         <f>0.0051*S37^3+0.5152*S37*S37+2.0815*S37-0.5714</f>
         <v>63.611200000000011</v>
       </c>
-      <c r="V37">
-        <f>1.9579*S37^1.553</f>
-        <v>59.39216046080093</v>
-      </c>
     </row>
-    <row r="38" spans="19:22">
+    <row r="38" spans="19:21">
       <c r="S38">
         <v>10</v>
       </c>
@@ -6617,10 +6619,6 @@
       <c r="U38">
         <f>0.0051*S38^3+0.5152*S38*S38+2.0815*S38-0.5714</f>
         <v>76.863600000000005</v>
-      </c>
-      <c r="V38">
-        <f>1.9579*S38^1.553</f>
-        <v>69.950448981766172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>